<commit_message>
Added readCSV file to input states get functions for states and districts
</commit_message>
<xml_diff>
--- a/DataStructuresProject3/District_map.xlsx
+++ b/DataStructuresProject3/District_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maura Elosegui\source\repos\539\DataStructuresProject3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74105D0B-F042-4C4B-97B3-051A9579C948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD849BD-0939-471E-8CBB-06B3E2848543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="6300" windowWidth="18000" windowHeight="11055" xr2:uid="{B576BF06-D8E7-4931-8545-D57E9AAA9B99}"/>
+    <workbookView xWindow="96" yWindow="912" windowWidth="11268" windowHeight="10968" xr2:uid="{B576BF06-D8E7-4931-8545-D57E9AAA9B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Number of Districts</t>
   </si>
@@ -51,9 +51,6 @@
     <t>% REP</t>
   </si>
   <si>
-    <t>% OTHER</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -67,6 +64,45 @@
   </si>
   <si>
     <t>True Turnout</t>
+  </si>
+  <si>
+    <t>Dem Senator</t>
+  </si>
+  <si>
+    <t>Rep Senator</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Dem Rep</t>
+  </si>
+  <si>
+    <t>Rep Rep</t>
+  </si>
+  <si>
+    <t>Dina Titus</t>
+  </si>
+  <si>
+    <t>Joyce Bentley</t>
+  </si>
+  <si>
+    <t>Patricia Ackerman</t>
+  </si>
+  <si>
+    <t>Mark E. Amodei</t>
+  </si>
+  <si>
+    <t>Suzzanne Lee</t>
+  </si>
+  <si>
+    <t>Dan Rodimer</t>
+  </si>
+  <si>
+    <t>Steven A. Horsford</t>
+  </si>
+  <si>
+    <t>Jim Marchant</t>
   </si>
 </sst>
 </file>
@@ -428,87 +464,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBEAA11-795E-4093-A04F-1DFE9E42F9C1}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="17" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2">
-        <v>159544854</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="2">
+        <v>159544854</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2">
         <v>160000</v>
       </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>3</v>
@@ -517,100 +563,135 @@
         <v>4</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <f>ROUNDDOWN(1407754/C1*E1,0)</f>
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f>ROUNDDOWN(1407754/E1*G1,0)</f>
         <v>1411</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <f>ROUNDDOWN((137868+74490+6190+4665)/C1*E1,0)</f>
+      <c r="G3">
+        <f>ROUNDDOWN((137868+74490+6190+4665)/E1*G1,0)</f>
         <v>223</v>
       </c>
-      <c r="F3">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
         <v>0.61799999999999999</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>0.33400000000000002</v>
       </c>
-      <c r="H3">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="I3">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="J3">
-        <f>ROUNDDOWN((216078+155780+10815)/C1*E1,0)</f>
+      <c r="M3">
+        <f>ROUNDDOWN((216078+155780+10815)/E1*G1,0)</f>
         <v>383</v>
       </c>
-      <c r="K3">
+      <c r="N3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3">
         <v>0.40699999999999997</v>
       </c>
-      <c r="L3">
+      <c r="Q3">
         <v>0.56499999999999995</v>
       </c>
-      <c r="M3">
-        <v>2.8299999999999999E-2</v>
-      </c>
-      <c r="N3">
+      <c r="R3">
         <v>3</v>
       </c>
-      <c r="O3">
-        <f>ROUNDDOWN((203421+190975+12315+10541)/C1*E1,0)</f>
+      <c r="S3">
+        <f>ROUNDDOWN((203421+190975+12315+10541)/E1*G1,0)</f>
         <v>418</v>
       </c>
-      <c r="P3">
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3">
         <v>0.48799999999999999</v>
       </c>
-      <c r="Q3">
+      <c r="W3">
         <v>0.45800000000000002</v>
       </c>
-      <c r="R3">
-        <f>1-(P3+Q3)</f>
-        <v>5.4000000000000048E-2</v>
-      </c>
-      <c r="S3">
+      <c r="X3">
         <v>4</v>
       </c>
-      <c r="T3">
-        <f>B3-(O3+E3+J3)</f>
+      <c r="Y3">
+        <f>D3-(S3+G3+M3)</f>
         <v>387</v>
       </c>
-      <c r="U3">
+      <c r="Z3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB3">
         <v>0.50700000000000001</v>
       </c>
-      <c r="V3">
+      <c r="AC3">
         <v>0.45800000000000002</v>
-      </c>
-      <c r="W3">
-        <f>1-(U3+V3)</f>
-        <v>3.499999999999992E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to unordered maps Added Idaho to CSV, functions didn't break
</commit_message>
<xml_diff>
--- a/DataStructuresProject3/District_map.xlsx
+++ b/DataStructuresProject3/District_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maura Elosegui\source\repos\539\DataStructuresProject3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\source\repos\DataStructuresProject3\DataStructuresProject3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD849BD-0939-471E-8CBB-06B3E2848543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42588BAC-0813-4CAD-B5C1-2CE68E024314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="912" windowWidth="11268" windowHeight="10968" xr2:uid="{B576BF06-D8E7-4931-8545-D57E9AAA9B99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B576BF06-D8E7-4931-8545-D57E9AAA9B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Number of Districts</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>Jim Marchant</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Paulette Jordan</t>
+  </si>
+  <si>
+    <t>Jim Risch</t>
+  </si>
+  <si>
+    <t>Rudy Soto</t>
+  </si>
+  <si>
+    <t>Russ Fulcher</t>
+  </si>
+  <si>
+    <t>C. Aaron Swisher</t>
+  </si>
+  <si>
+    <t>Mike Simpson</t>
+  </si>
+  <si>
+    <t>Electoral Votes</t>
   </si>
 </sst>
 </file>
@@ -146,10 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,53 +489,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBEAA11-795E-4093-A04F-1DFE9E42F9C1}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="17" customWidth="1"/>
-    <col min="24" max="24" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2">
+      <c r="F1" s="2">
         <v>159544854</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2">
+      <c r="H1" s="2">
         <v>160000</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -524,173 +550,251 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUNDDOWN((875000/F1)*H1,0)</f>
+        <v>877</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <f>ROUNDDOWN(458569/F1*H1,0)</f>
+        <v>459</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3">
+        <f>ROUNDDOWN(391333/F1*H1,0)</f>
+        <v>392</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.317</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <f>ROUNDDOWN(1407754/E1*G1,0)</f>
+      <c r="D4">
+        <f>ROUNDDOWN((1407754/F1)*H1,0)</f>
         <v>1411</v>
       </c>
-      <c r="E3">
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G3">
-        <f>ROUNDDOWN((137868+74490+6190+4665)/E1*G1,0)</f>
+      <c r="H4">
+        <f>ROUNDDOWN((137868+74490+6190+4665)/F1*H1,0)</f>
         <v>223</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="J3">
+      <c r="K4">
         <v>0.61799999999999999</v>
       </c>
-      <c r="K3">
+      <c r="L4">
         <v>0.33400000000000002</v>
       </c>
-      <c r="L3">
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="M3">
-        <f>ROUNDDOWN((216078+155780+10815)/E1*G1,0)</f>
+      <c r="N4">
+        <f>ROUNDDOWN((216078+155780+10815)/F1*H1,0)</f>
         <v>383</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O4" t="s">
         <v>17</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P4" t="s">
         <v>18</v>
       </c>
-      <c r="P3">
+      <c r="Q4">
         <v>0.40699999999999997</v>
       </c>
-      <c r="Q3">
+      <c r="R4">
         <v>0.56499999999999995</v>
       </c>
-      <c r="R3">
+      <c r="S4">
         <v>3</v>
       </c>
-      <c r="S3">
-        <f>ROUNDDOWN((203421+190975+12315+10541)/E1*G1,0)</f>
+      <c r="T4">
+        <f>ROUNDDOWN((203421+190975+12315+10541)/F1*H1,0)</f>
         <v>418</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U4" t="s">
         <v>19</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V4" t="s">
         <v>20</v>
       </c>
-      <c r="V3">
+      <c r="W4">
         <v>0.48799999999999999</v>
       </c>
-      <c r="W3">
+      <c r="X4">
         <v>0.45800000000000002</v>
       </c>
-      <c r="X3">
+      <c r="Y4">
         <v>4</v>
       </c>
-      <c r="Y3">
-        <f>D3-(S3+G3+M3)</f>
+      <c r="Z4">
+        <f>D4-(T4+H4+N4)</f>
         <v>387</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA4" t="s">
         <v>21</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB4" t="s">
         <v>22</v>
       </c>
-      <c r="AB3">
+      <c r="AC4">
         <v>0.50700000000000001</v>
       </c>
-      <c r="AC3">
+      <c r="AD4">
         <v>0.45800000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Columns for percentages
National and Senate percentages columns added
</commit_message>
<xml_diff>
--- a/DataStructuresProject3/District_map.xlsx
+++ b/DataStructuresProject3/District_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\source\repos\DataStructuresProject3\DataStructuresProject3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\539\DataStructuresProject3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42588BAC-0813-4CAD-B5C1-2CE68E024314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1603AC41-AC87-4C3A-AC1A-DB45E254028C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B576BF06-D8E7-4931-8545-D57E9AAA9B99}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B576BF06-D8E7-4931-8545-D57E9AAA9B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>Number of Districts</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Electoral Votes</t>
+  </si>
+  <si>
+    <t>% DEM Sen</t>
+  </si>
+  <si>
+    <t>% REP Sen</t>
+  </si>
+  <si>
+    <t>% DEM Nat</t>
+  </si>
+  <si>
+    <t>% REP Nat</t>
   </si>
 </sst>
 </file>
@@ -489,35 +501,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBEAA11-795E-4093-A04F-1DFE9E42F9C1}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="18.44140625" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17" customWidth="1"/>
+    <col min="17" max="17" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="7.33203125" customWidth="1"/>
+    <col min="23" max="23" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="17" customWidth="1"/>
+    <col min="29" max="29" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -527,16 +540,20 @@
       <c r="F1" s="2">
         <v>159544854</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2">
-        <v>160000</v>
-      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2">
+        <v>160000</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -556,80 +573,92 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="1"/>
+      <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -640,7 +669,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="3">
-        <f>ROUNDDOWN((875000/F1)*H1,0)</f>
+        <f>ROUNDDOWN((875000/F1)*L1,0)</f>
         <v>877</v>
       </c>
       <c r="E3" s="3">
@@ -650,47 +679,55 @@
         <v>2</v>
       </c>
       <c r="G3" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="K3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
-        <f>ROUNDDOWN(458569/F1*H1,0)</f>
+      <c r="L3" s="3">
+        <f>ROUNDDOWN(458569/F1*L1,0)</f>
         <v>459</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="3">
+      <c r="O3" s="3">
         <v>0.28699999999999998</v>
       </c>
-      <c r="L3" s="3">
+      <c r="P3" s="3">
         <v>0.67800000000000005</v>
       </c>
-      <c r="M3" s="3">
+      <c r="Q3" s="3">
         <v>2</v>
       </c>
-      <c r="N3" s="3">
-        <f>ROUNDDOWN(391333/F1*H1,0)</f>
+      <c r="R3" s="3">
+        <f>ROUNDDOWN(391333/F1*L1,0)</f>
         <v>392</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="U3" s="3">
         <v>0.317</v>
       </c>
-      <c r="R3" s="3">
+      <c r="V3" s="3">
         <v>0.64100000000000001</v>
       </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
@@ -699,9 +736,13 @@
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-      <c r="AE3" s="1"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -712,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <f>ROUNDDOWN((1407754/F1)*H1,0)</f>
+        <f>ROUNDDOWN((1407754/F1)*L1,0)</f>
         <v>1411</v>
       </c>
       <c r="E4">
@@ -722,81 +763,102 @@
         <v>4</v>
       </c>
       <c r="G4">
+        <v>0.1</v>
+      </c>
+      <c r="H4">
+        <v>0.11</v>
+      </c>
+      <c r="I4">
+        <v>0.11</v>
+      </c>
+      <c r="J4">
+        <v>0.1</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="H4">
-        <f>ROUNDDOWN((137868+74490+6190+4665)/F1*H1,0)</f>
+      <c r="L4">
+        <f>ROUNDDOWN((137868+74490+6190+4665)/F1*L1,0)</f>
         <v>223</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>16</v>
       </c>
-      <c r="K4">
+      <c r="O4">
         <v>0.61799999999999999</v>
       </c>
-      <c r="L4">
+      <c r="P4">
         <v>0.33400000000000002</v>
       </c>
-      <c r="M4">
+      <c r="Q4">
         <v>2</v>
       </c>
-      <c r="N4">
-        <f>ROUNDDOWN((216078+155780+10815)/F1*H1,0)</f>
+      <c r="R4">
+        <f>ROUNDDOWN((216078+155780+10815)/F1*L1,0)</f>
         <v>383</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
         <v>17</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>18</v>
       </c>
-      <c r="Q4">
+      <c r="U4">
         <v>0.40699999999999997</v>
       </c>
-      <c r="R4">
+      <c r="V4">
         <v>0.56499999999999995</v>
       </c>
-      <c r="S4">
+      <c r="W4">
         <v>3</v>
       </c>
-      <c r="T4">
-        <f>ROUNDDOWN((203421+190975+12315+10541)/F1*H1,0)</f>
+      <c r="X4">
+        <f>ROUNDDOWN((203421+190975+12315+10541)/F1*L1,0)</f>
         <v>418</v>
       </c>
-      <c r="U4" t="s">
+      <c r="Y4" t="s">
         <v>19</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Z4" t="s">
         <v>20</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>0.48799999999999999</v>
       </c>
-      <c r="X4">
+      <c r="AB4">
         <v>0.45800000000000002</v>
       </c>
-      <c r="Y4">
+      <c r="AC4">
         <v>4</v>
       </c>
-      <c r="Z4">
-        <f>D4-(T4+H4+N4)</f>
+      <c r="AD4">
+        <f>D4-(X4+L4+R4)</f>
         <v>387</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AE4" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AF4" t="s">
         <v>22</v>
       </c>
-      <c r="AC4">
+      <c r="AG4">
         <v>0.50700000000000001</v>
       </c>
-      <c r="AD4">
+      <c r="AH4">
         <v>0.45800000000000002</v>
       </c>
+    </row>
+    <row r="28" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>